<commit_message>
altera coisas simples no código
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -574,7 +574,27 @@
           <t>awdawd</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" t="n">
+        <v>1234567890123</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>aaadw</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>adawd</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>awdawd</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
         <is>
           <t>1234567890123</t>
         </is>
@@ -591,14 +611,77 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>nome</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>idade</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>cpf</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>telefone</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>endereco</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>abc</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>123</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>12345678901</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>abcde@gmail.com</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>1212341234</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>rua1</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>